<commit_message>
Updated Project Plan, added canvas to LaurenScene
</commit_message>
<xml_diff>
--- a/TeamOne-FinalProjectPlan.xlsx
+++ b/TeamOne-FinalProjectPlan.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SWE0227\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\__Wake Tech SGD\_2019 Fall Semester\Software Development\Team One Final Project\November 6\teamOne-Pirates-repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Project Plan" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="31">
   <si>
     <t>Estimated Implementation</t>
   </si>
@@ -114,6 +114,9 @@
   </si>
   <si>
     <t>Group effort</t>
+  </si>
+  <si>
+    <t>Find Player model, add all animations</t>
   </si>
 </sst>
 </file>
@@ -479,10 +482,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -553,7 +556,7 @@
         <v>11</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -567,7 +570,7 @@
         <v>13</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -581,32 +584,32 @@
         <v>15</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="8" t="s">
-        <v>16</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="B10" s="7">
-        <v>43782</v>
+        <v>43775</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
-        <v>17</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="8" t="s">
+        <v>16</v>
       </c>
       <c r="B11" s="7">
         <v>43782</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>3</v>
@@ -614,13 +617,13 @@
     </row>
     <row r="12" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B12" s="7">
         <v>43782</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>3</v>
@@ -628,27 +631,27 @@
     </row>
     <row r="13" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B13" s="7">
-        <v>43789</v>
+        <v>43782</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="B14" s="7">
         <v>43789</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>3</v>
@@ -656,7 +659,7 @@
     </row>
     <row r="15" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B15" s="7">
         <v>43789</v>
@@ -670,27 +673,27 @@
     </row>
     <row r="16" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B16" s="7">
-        <v>43794</v>
+        <v>43789</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B17" s="7">
         <v>43794</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>3</v>
@@ -698,7 +701,7 @@
     </row>
     <row r="18" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B18" s="7">
         <v>43794</v>
@@ -712,7 +715,7 @@
     </row>
     <row r="19" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B19" s="7">
         <v>43794</v>
@@ -726,10 +729,10 @@
     </row>
     <row r="20" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B20" s="7">
-        <v>43805</v>
+        <v>43794</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>11</v>
@@ -740,13 +743,13 @@
     </row>
     <row r="21" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B21" s="7">
         <v>43805</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>3</v>
@@ -754,23 +757,31 @@
     </row>
     <row r="22" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B22" s="7">
         <v>43805</v>
       </c>
       <c r="C22" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23" s="7">
+        <v>43805</v>
+      </c>
+      <c r="C23" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D22" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="3"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="3"/>
+      <c r="D23" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="24" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3"/>
@@ -778,19 +789,25 @@
       <c r="C24" s="4"/>
       <c r="D24" s="3"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
+    <row r="25" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="3"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="3"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
   <dataConsolidate/>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D7:D24">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D7:D25">
       <formula1>$D$4:$D$6</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Estimated completion date" prompt="Enter the expected due date for the feature." sqref="B3 B7:B24"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Who is in charge of the feature?" prompt="Enter the name of the teammate who is lead for the feature." sqref="C3 C7:C24"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Estimated completion date" prompt="Enter the expected due date for the feature." sqref="B3 B7:B25"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Who is in charge of the feature?" prompt="Enter the name of the teammate who is lead for the feature." sqref="C3 C7:C25"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Status" prompt="Use the dropdown menu to choose: Not implemented, In Progress or Done." sqref="D3"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fixed script issues and added some shooting elements
</commit_message>
<xml_diff>
--- a/TeamOne-FinalProjectPlan.xlsx
+++ b/TeamOne-FinalProjectPlan.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\__Wake Tech SGD\_2019 Fall Semester\Software Development\Team One Final Project\November 6\teamOne-Pirates-repo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Fletcher\teamOne-Pirates-repo\teamOne-Pirates-repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -123,7 +123,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -144,13 +144,49 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -177,10 +213,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -202,8 +241,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="4">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -484,8 +529,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -545,7 +590,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
@@ -555,11 +600,11 @@
       <c r="C7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>12</v>
       </c>
@@ -569,11 +614,11 @@
       <c r="C8" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>14</v>
       </c>
@@ -583,11 +628,11 @@
       <c r="C9" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>30</v>
       </c>
@@ -597,11 +642,11 @@
       <c r="C10" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>16</v>
       </c>
@@ -611,11 +656,11 @@
       <c r="C11" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="11" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>17</v>
       </c>
@@ -625,11 +670,11 @@
       <c r="C12" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D12" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>18</v>
       </c>
@@ -639,11 +684,11 @@
       <c r="C13" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>26</v>
       </c>
@@ -653,11 +698,11 @@
       <c r="C14" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="11" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>19</v>
       </c>
@@ -667,11 +712,11 @@
       <c r="C15" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D15" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D15" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>20</v>
       </c>
@@ -681,11 +726,11 @@
       <c r="C16" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D16" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>21</v>
       </c>
@@ -695,11 +740,11 @@
       <c r="C17" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D17" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D17" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>22</v>
       </c>
@@ -709,11 +754,11 @@
       <c r="C18" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D18" s="11" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>25</v>
       </c>
@@ -723,11 +768,11 @@
       <c r="C19" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D19" s="11" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>24</v>
       </c>
@@ -737,11 +782,11 @@
       <c r="C20" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D20" s="11" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>27</v>
       </c>
@@ -751,11 +796,11 @@
       <c r="C21" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D21" s="11" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>23</v>
       </c>
@@ -765,11 +810,11 @@
       <c r="C22" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D22" s="11" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>28</v>
       </c>
@@ -779,7 +824,7 @@
       <c r="C23" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="D23" s="11" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>